<commit_message>
Added pdf of schematic
</commit_message>
<xml_diff>
--- a/extension_board_v2/BOM_final.xlsx
+++ b/extension_board_v2/BOM_final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\elesensehw\hardware\converter-design-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\elesensehw\hardware\extension_board_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="PCB_Project3" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PCB_Project3!$A$1:$J$79</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="324">
   <si>
     <t>Comment</t>
   </si>
@@ -879,13 +880,133 @@
   </si>
   <si>
     <t>1K8/805, 1K8/805</t>
+  </si>
+  <si>
+    <t>MPN</t>
+  </si>
+  <si>
+    <t>smd capaciteit, verp.0603, 100nF, smd capaciteit, verp.0603, 12nF</t>
+  </si>
+  <si>
+    <t>C01CPU, C001LO, C02CPU, C002LO, C03CPU, C003LO, C004LO, C005LO, C06CPU, C006LO, C09CPU, C10CPU, C019LO, C029LO, C031LO, C34LO, C035LO, C49, C51, C74HF</t>
+  </si>
+  <si>
+    <t>CSMD603/100nF, CSMD603/12nF</t>
+  </si>
+  <si>
+    <t>C001Mx, C002Mx, C006Mx, C007Mx</t>
+  </si>
+  <si>
+    <t>C002BPMx</t>
+  </si>
+  <si>
+    <t>C003Mx, C009Mx</t>
+  </si>
+  <si>
+    <t>C004Mx, C008Mx</t>
+  </si>
+  <si>
+    <t>C005Mx, C010Mx, C014LO, C015LO, C016LO</t>
+  </si>
+  <si>
+    <t>C007LO, C017LO, C52, C56</t>
+  </si>
+  <si>
+    <t>C59, C67</t>
+  </si>
+  <si>
+    <t>smd capaciteit, verp.0603, 100pF, smd capaciteit, verp.0603, 10pF</t>
+  </si>
+  <si>
+    <t>C70, C71, C72, C76HF, C78HF, C79HF, C82HF, C83HF</t>
+  </si>
+  <si>
+    <t>CSMD603/100pF, CSMD603/10pF</t>
+  </si>
+  <si>
+    <t>D2, D3, D5</t>
+  </si>
+  <si>
+    <t>MOUNTHOLE_3MM</t>
+  </si>
+  <si>
+    <t>H1, H2, H3, H4</t>
+  </si>
+  <si>
+    <t>MOUNT_3MM</t>
+  </si>
+  <si>
+    <t>HIGH, LOW, MID, SDR1</t>
+  </si>
+  <si>
+    <t>CON SMD USB Micro MOLEX</t>
+  </si>
+  <si>
+    <t>MOLEX - 47589-0001 - MICRO USB TYPE AB</t>
+  </si>
+  <si>
+    <t>JUSB</t>
+  </si>
+  <si>
+    <t>SMD USB MOLEX</t>
+  </si>
+  <si>
+    <t>L01CPU, L5HF</t>
+  </si>
+  <si>
+    <t>L5Mx, L7Mx</t>
+  </si>
+  <si>
+    <t>weerstand SMD603, 470R</t>
+  </si>
+  <si>
+    <t>R01CPU</t>
+  </si>
+  <si>
+    <t>470R/603</t>
+  </si>
+  <si>
+    <t>R02CPU, R03CPU, R04CPU</t>
+  </si>
+  <si>
+    <t>weerstand SMD805, 270R, weerstand SMD805, 1K8</t>
+  </si>
+  <si>
+    <t>R002LO, R040LO, R041LO</t>
+  </si>
+  <si>
+    <t>270R/805, 1K8/805</t>
+  </si>
+  <si>
+    <t>50R/402</t>
+  </si>
+  <si>
+    <t>weerstand SMD402, 50R</t>
+  </si>
+  <si>
+    <t>22R/Network4/603</t>
+  </si>
+  <si>
+    <t>weerstand SMD603, 22R, weerstand SMD603, 750R, weerstand SMD603, 51R</t>
+  </si>
+  <si>
+    <t>R07CPU, R08CPU, R28, R30, R32, R34HF, R37HF, R38HF</t>
+  </si>
+  <si>
+    <t>22R/603, 750R/603, 51R/603</t>
+  </si>
+  <si>
+    <t>U13</t>
+  </si>
+  <si>
+    <t>U20, U31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -907,13 +1028,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -922,7 +1036,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -938,11 +1052,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -981,11 +1090,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -999,17 +1107,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1289,10 +1396,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,7 +1414,7 @@
     <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1339,7 +1446,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1367,8 +1474,11 @@
       <c r="I2" s="7">
         <v>2725755</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>2691054</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1397,7 +1507,7 @@
         <v>2320813</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1426,7 +1536,7 @@
         <v>2627341</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1455,7 +1565,7 @@
         <v>2522382</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1484,7 +1594,7 @@
         <v>1414601</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
@@ -1513,7 +1623,7 @@
         <v>2310297</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
@@ -1542,7 +1652,7 @@
         <v>1650837</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
@@ -1571,7 +1681,7 @@
         <v>2776894</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
@@ -1600,7 +1710,7 @@
         <v>2218849</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -1629,7 +1739,7 @@
         <v>1828887</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
@@ -1658,7 +1768,7 @@
         <v>1907314</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -1687,7 +1797,7 @@
         <v>1865466</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -1716,7 +1826,7 @@
         <v>2496915</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>57</v>
       </c>
@@ -1742,7 +1852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>57</v>
       </c>
@@ -1820,7 +1930,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>70</v>
       </c>
@@ -1849,7 +1959,7 @@
         <v>2496792</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>72</v>
       </c>
@@ -1878,7 +1988,7 @@
         <v>2781463</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>74</v>
       </c>
@@ -1907,7 +2017,7 @@
         <v>1759062</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>78</v>
       </c>
@@ -1936,7 +2046,7 @@
         <v>1535558</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>81</v>
       </c>
@@ -2020,7 +2130,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>89</v>
       </c>
@@ -2049,7 +2159,7 @@
         <v>1791462</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>91</v>
       </c>
@@ -2104,7 +2214,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>97</v>
       </c>
@@ -2133,7 +2243,7 @@
         <v>1248989</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>102</v>
       </c>
@@ -2162,7 +2272,7 @@
         <v>1669753</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>107</v>
       </c>
@@ -2191,7 +2301,7 @@
         <v>2286003</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>110</v>
       </c>
@@ -2220,7 +2330,7 @@
         <v>2286389</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>113</v>
       </c>
@@ -2249,7 +2359,7 @@
         <v>2286389</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>117</v>
       </c>
@@ -2276,7 +2386,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>120</v>
       </c>
@@ -2305,7 +2415,7 @@
         <v>2497374</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>123</v>
       </c>
@@ -2334,7 +2444,7 @@
         <v>2497355</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>126</v>
       </c>
@@ -2389,7 +2499,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>134</v>
       </c>
@@ -2444,53 +2554,53 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11" t="s">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="E41" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="F41" s="12">
-        <v>1</v>
-      </c>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
+      <c r="F41" s="11">
+        <v>1</v>
+      </c>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
       <c r="I41" s="7">
         <v>9334254</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11" t="s">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="10" t="s">
         <v>283</v>
       </c>
       <c r="F42">
         <v>2</v>
       </c>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
       <c r="I42" s="7">
         <v>2447595</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>141</v>
       </c>
@@ -2519,7 +2629,7 @@
         <v>1697424</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>145</v>
       </c>
@@ -2548,7 +2658,7 @@
         <v>2447183</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>150</v>
       </c>
@@ -2577,36 +2687,36 @@
         <v>2447279</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="D46" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="E46" s="10" t="s">
         <v>278</v>
       </c>
       <c r="F46">
         <v>1</v>
       </c>
-      <c r="G46" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H46" s="11" t="s">
+      <c r="G46" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46" s="10" t="s">
         <v>9</v>
       </c>
       <c r="I46">
         <v>2060088</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>157</v>
       </c>
@@ -2635,7 +2745,7 @@
         <v>2059275</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>161</v>
       </c>
@@ -2664,7 +2774,7 @@
         <v>2447305</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>165</v>
       </c>
@@ -2693,7 +2803,7 @@
         <v>1170635</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>167</v>
       </c>
@@ -2722,7 +2832,7 @@
         <v>2309112</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>150</v>
       </c>
@@ -2751,7 +2861,7 @@
         <v>2447592</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>172</v>
       </c>
@@ -2780,7 +2890,7 @@
         <v>2447230</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>176</v>
       </c>
@@ -2809,7 +2919,7 @@
         <v>2502455</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>180</v>
       </c>
@@ -2864,7 +2974,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>186</v>
       </c>
@@ -2893,7 +3003,7 @@
         <v>2324285</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>189</v>
       </c>
@@ -2922,7 +3032,7 @@
         <v>2360869</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>195</v>
       </c>
@@ -2951,7 +3061,7 @@
         <v>1081242</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>199</v>
       </c>
@@ -3058,7 +3168,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>213</v>
       </c>
@@ -3113,7 +3223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>220</v>
       </c>
@@ -3145,7 +3255,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>224</v>
       </c>
@@ -3174,7 +3284,7 @@
         <v>1506629</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>228</v>
       </c>
@@ -3203,7 +3313,7 @@
         <v>1467776</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>231</v>
       </c>
@@ -3232,7 +3342,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>234</v>
       </c>
@@ -3261,7 +3371,7 @@
         <v>2066354</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>240</v>
       </c>
@@ -3290,7 +3400,7 @@
         <v>2506414</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>242</v>
       </c>
@@ -3319,7 +3429,7 @@
         <v>1903303</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>245</v>
       </c>
@@ -3348,7 +3458,7 @@
         <v>2212081</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>248</v>
       </c>
@@ -3377,7 +3487,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>253</v>
       </c>
@@ -3406,7 +3516,7 @@
         <v>2377140</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>88</v>
       </c>
@@ -3435,7 +3545,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>260</v>
       </c>
@@ -3464,7 +3574,7 @@
         <v>2112373</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>262</v>
       </c>
@@ -3493,7 +3603,7 @@
         <v>2545845</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>264</v>
       </c>
@@ -3518,11 +3628,14 @@
       <c r="H78" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I78" s="10"/>
+      <c r="I78" s="7">
+        <v>2854044</v>
+      </c>
       <c r="J78" s="7" t="s">
         <v>276</v>
       </c>
     </row>
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:J79">
     <filterColumn colId="0">
@@ -3588,6 +3701,11 @@
         <filter val="TCA6408A"/>
         <filter val="USB-B"/>
         <filter val="X1G004691000112"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="8">
+      <filters>
+        <filter val="2691054"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3656,8 +3774,1519 @@
     <hyperlink ref="I56" r:id="rId62" tooltip="2324285" display="http://be.farnell.com/panasonic-electronic-components/erj2gej200x/res-thick-film-20r-5-0-1w-0402/dp/2324285"/>
     <hyperlink ref="I42" r:id="rId63" tooltip="2447595" display="http://be.farnell.com/multicomp/mcwr08x1801ftl/res-thick-film-1k8-1-0-125w-0805/dp/2447595?st=resistor%201.8k%200805"/>
     <hyperlink ref="I41" r:id="rId64" tooltip="9334254" display="http://be.farnell.com/multicomp/mc01w08055270r/res-thick-film-270r-5-0-1w-0805/dp/9334254?st=resistor%201.8k%200805"/>
+    <hyperlink ref="I78" r:id="rId65" display="https://be.farnell.com/multicomp/mcsjk-7i-16-00-18-10-60-b-10/crystal-16mhz-18pf-5mm-x-3-2mm/dp/2854044?st=MCSJK-7I-16.00-18-10-60-B-10%20-%20%20Crystal,%2016%20MHz,%20SMD,%205mm%20x%203.2mm,%2010%20ppm,%2018%20pF,%2010%20ppm"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId65"/>
+  <pageSetup orientation="portrait" r:id="rId66"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="87.42578125" customWidth="1"/>
+    <col min="4" max="9" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="9">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="F3" s="9">
+        <v>20</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="9">
+        <v>5</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="9">
+        <v>2</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="9">
+        <v>2</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="9">
+        <v>2</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="9">
+        <v>5</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="9">
+        <v>2</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="9">
+        <v>4</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="9">
+        <v>7</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="9">
+        <v>5</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="9">
+        <v>1</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="9">
+        <v>2</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="9">
+        <v>1</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="F18" s="9">
+        <v>8</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="9">
+        <v>1</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="9">
+        <v>1</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="9">
+        <v>1</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="9">
+        <v>1</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="9">
+        <v>3</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="9">
+        <v>1</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F25" s="9">
+        <v>4</v>
+      </c>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="9">
+        <v>4</v>
+      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="F27" s="9">
+        <v>1</v>
+      </c>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" s="9">
+        <v>2</v>
+      </c>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F29" s="9">
+        <v>1</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F30" s="9">
+        <v>2</v>
+      </c>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F31" s="9">
+        <v>5</v>
+      </c>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F32" s="9">
+        <v>1</v>
+      </c>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F33" s="9">
+        <v>1</v>
+      </c>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F34" s="9">
+        <v>1</v>
+      </c>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="F35" s="9">
+        <v>1</v>
+      </c>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F36" s="9">
+        <v>1</v>
+      </c>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>750</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="F37" s="9">
+        <v>3</v>
+      </c>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="F38" s="9">
+        <v>3</v>
+      </c>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>270</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F39" s="9">
+        <v>1</v>
+      </c>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="F40" s="9">
+        <v>3</v>
+      </c>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F41" s="9">
+        <v>2</v>
+      </c>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="F42" s="9">
+        <v>1</v>
+      </c>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>51</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="F43" s="9">
+        <v>8</v>
+      </c>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="9">
+        <v>240</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F44" s="9">
+        <v>1</v>
+      </c>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="9">
+        <v>30.1</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F45" s="9">
+        <v>1</v>
+      </c>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="9">
+        <v>0</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F46" s="9">
+        <v>1</v>
+      </c>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="F47" s="9">
+        <v>2</v>
+      </c>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="9">
+        <v>390</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F48" s="9">
+        <v>1</v>
+      </c>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="9">
+        <v>91</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F49" s="9">
+        <v>1</v>
+      </c>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F50" s="9">
+        <v>1</v>
+      </c>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F51" s="9">
+        <v>1</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="I51" s="9"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="F52" s="9">
+        <v>1</v>
+      </c>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F53" s="9">
+        <v>1</v>
+      </c>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="F54" s="9">
+        <v>1</v>
+      </c>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="F55" s="9">
+        <v>1</v>
+      </c>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="F56" s="9">
+        <v>1</v>
+      </c>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="F57" s="9">
+        <v>1</v>
+      </c>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="F58" s="9">
+        <v>1</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="F59" s="9">
+        <v>1</v>
+      </c>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="F60" s="9">
+        <v>1</v>
+      </c>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="F61" s="9">
+        <v>1</v>
+      </c>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="F62" s="9">
+        <v>2</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="I62" s="9"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F63" s="9">
+        <v>1</v>
+      </c>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="F64" s="9">
+        <v>1</v>
+      </c>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="F65" s="9">
+        <v>1</v>
+      </c>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixing image rejection filter
</commit_message>
<xml_diff>
--- a/extension_board_v2/BOM_final.xlsx
+++ b/extension_board_v2/BOM_final.xlsx
@@ -13,7 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="PCB_Project3" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PCB_Project3!$A$1:$J$79</definedName>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="284">
   <si>
     <t>Comment</t>
   </si>
@@ -880,126 +879,6 @@
   </si>
   <si>
     <t>1K8/805, 1K8/805</t>
-  </si>
-  <si>
-    <t>MPN</t>
-  </si>
-  <si>
-    <t>smd capaciteit, verp.0603, 100nF, smd capaciteit, verp.0603, 12nF</t>
-  </si>
-  <si>
-    <t>C01CPU, C001LO, C02CPU, C002LO, C03CPU, C003LO, C004LO, C005LO, C06CPU, C006LO, C09CPU, C10CPU, C019LO, C029LO, C031LO, C34LO, C035LO, C49, C51, C74HF</t>
-  </si>
-  <si>
-    <t>CSMD603/100nF, CSMD603/12nF</t>
-  </si>
-  <si>
-    <t>C001Mx, C002Mx, C006Mx, C007Mx</t>
-  </si>
-  <si>
-    <t>C002BPMx</t>
-  </si>
-  <si>
-    <t>C003Mx, C009Mx</t>
-  </si>
-  <si>
-    <t>C004Mx, C008Mx</t>
-  </si>
-  <si>
-    <t>C005Mx, C010Mx, C014LO, C015LO, C016LO</t>
-  </si>
-  <si>
-    <t>C007LO, C017LO, C52, C56</t>
-  </si>
-  <si>
-    <t>C59, C67</t>
-  </si>
-  <si>
-    <t>smd capaciteit, verp.0603, 100pF, smd capaciteit, verp.0603, 10pF</t>
-  </si>
-  <si>
-    <t>C70, C71, C72, C76HF, C78HF, C79HF, C82HF, C83HF</t>
-  </si>
-  <si>
-    <t>CSMD603/100pF, CSMD603/10pF</t>
-  </si>
-  <si>
-    <t>D2, D3, D5</t>
-  </si>
-  <si>
-    <t>MOUNTHOLE_3MM</t>
-  </si>
-  <si>
-    <t>H1, H2, H3, H4</t>
-  </si>
-  <si>
-    <t>MOUNT_3MM</t>
-  </si>
-  <si>
-    <t>HIGH, LOW, MID, SDR1</t>
-  </si>
-  <si>
-    <t>CON SMD USB Micro MOLEX</t>
-  </si>
-  <si>
-    <t>MOLEX - 47589-0001 - MICRO USB TYPE AB</t>
-  </si>
-  <si>
-    <t>JUSB</t>
-  </si>
-  <si>
-    <t>SMD USB MOLEX</t>
-  </si>
-  <si>
-    <t>L01CPU, L5HF</t>
-  </si>
-  <si>
-    <t>L5Mx, L7Mx</t>
-  </si>
-  <si>
-    <t>weerstand SMD603, 470R</t>
-  </si>
-  <si>
-    <t>R01CPU</t>
-  </si>
-  <si>
-    <t>470R/603</t>
-  </si>
-  <si>
-    <t>R02CPU, R03CPU, R04CPU</t>
-  </si>
-  <si>
-    <t>weerstand SMD805, 270R, weerstand SMD805, 1K8</t>
-  </si>
-  <si>
-    <t>R002LO, R040LO, R041LO</t>
-  </si>
-  <si>
-    <t>270R/805, 1K8/805</t>
-  </si>
-  <si>
-    <t>50R/402</t>
-  </si>
-  <si>
-    <t>weerstand SMD402, 50R</t>
-  </si>
-  <si>
-    <t>22R/Network4/603</t>
-  </si>
-  <si>
-    <t>weerstand SMD603, 22R, weerstand SMD603, 750R, weerstand SMD603, 51R</t>
-  </si>
-  <si>
-    <t>R07CPU, R08CPU, R28, R30, R32, R34HF, R37HF, R38HF</t>
-  </si>
-  <si>
-    <t>22R/603, 750R/603, 51R/603</t>
-  </si>
-  <si>
-    <t>U13</t>
-  </si>
-  <si>
-    <t>U20, U31</t>
   </si>
 </sst>
 </file>
@@ -1095,7 +974,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1112,7 +991,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1396,10 +1274,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,7 +1292,7 @@
     <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1446,7 +1324,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1474,11 +1352,8 @@
       <c r="I2" s="7">
         <v>2725755</v>
       </c>
-      <c r="K2">
-        <v>2691054</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1507,7 +1382,7 @@
         <v>2320813</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1536,7 +1411,7 @@
         <v>2627341</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1565,7 +1440,7 @@
         <v>2522382</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1594,7 +1469,7 @@
         <v>1414601</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
@@ -1623,7 +1498,7 @@
         <v>2310297</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
@@ -1652,7 +1527,7 @@
         <v>1650837</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
@@ -1681,7 +1556,7 @@
         <v>2776894</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
@@ -1710,7 +1585,7 @@
         <v>2218849</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -1739,7 +1614,7 @@
         <v>1828887</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
@@ -1768,7 +1643,7 @@
         <v>1907314</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -1797,7 +1672,7 @@
         <v>1865466</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -1826,7 +1701,7 @@
         <v>2496915</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>57</v>
       </c>
@@ -1852,7 +1727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>57</v>
       </c>
@@ -1930,7 +1805,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>70</v>
       </c>
@@ -1959,7 +1834,7 @@
         <v>2496792</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>72</v>
       </c>
@@ -1988,7 +1863,7 @@
         <v>2781463</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>74</v>
       </c>
@@ -2017,7 +1892,7 @@
         <v>1759062</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>78</v>
       </c>
@@ -2046,7 +1921,7 @@
         <v>1535558</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>81</v>
       </c>
@@ -2130,7 +2005,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>89</v>
       </c>
@@ -2159,7 +2034,7 @@
         <v>1791462</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>91</v>
       </c>
@@ -2214,7 +2089,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>97</v>
       </c>
@@ -2243,7 +2118,7 @@
         <v>1248989</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>102</v>
       </c>
@@ -2272,7 +2147,7 @@
         <v>1669753</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>107</v>
       </c>
@@ -2301,7 +2176,7 @@
         <v>2286003</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>110</v>
       </c>
@@ -2330,7 +2205,7 @@
         <v>2286389</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>113</v>
       </c>
@@ -2359,7 +2234,7 @@
         <v>2286389</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>117</v>
       </c>
@@ -2386,7 +2261,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>120</v>
       </c>
@@ -2415,7 +2290,7 @@
         <v>2497374</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>123</v>
       </c>
@@ -2444,7 +2319,7 @@
         <v>2497355</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>126</v>
       </c>
@@ -2499,7 +2374,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>134</v>
       </c>
@@ -2554,7 +2429,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="10" t="s">
         <v>142</v>
@@ -2577,7 +2452,7 @@
         <v>9334254</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="10" t="s">
         <v>280</v>
@@ -2600,7 +2475,7 @@
         <v>2447595</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>141</v>
       </c>
@@ -2629,7 +2504,7 @@
         <v>1697424</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>145</v>
       </c>
@@ -2658,7 +2533,7 @@
         <v>2447183</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>150</v>
       </c>
@@ -2687,7 +2562,7 @@
         <v>2447279</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>277</v>
       </c>
@@ -2716,7 +2591,7 @@
         <v>2060088</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>157</v>
       </c>
@@ -2745,7 +2620,7 @@
         <v>2059275</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>161</v>
       </c>
@@ -2774,7 +2649,7 @@
         <v>2447305</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>165</v>
       </c>
@@ -2803,7 +2678,7 @@
         <v>1170635</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>167</v>
       </c>
@@ -2832,7 +2707,7 @@
         <v>2309112</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>150</v>
       </c>
@@ -2861,7 +2736,7 @@
         <v>2447592</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>172</v>
       </c>
@@ -2890,7 +2765,7 @@
         <v>2447230</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>176</v>
       </c>
@@ -2919,7 +2794,7 @@
         <v>2502455</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>180</v>
       </c>
@@ -2974,7 +2849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>186</v>
       </c>
@@ -3003,7 +2878,7 @@
         <v>2324285</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>189</v>
       </c>
@@ -3032,7 +2907,7 @@
         <v>2360869</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>195</v>
       </c>
@@ -3061,7 +2936,7 @@
         <v>1081242</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>199</v>
       </c>
@@ -3168,7 +3043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>213</v>
       </c>
@@ -3223,7 +3098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>220</v>
       </c>
@@ -3255,7 +3130,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>224</v>
       </c>
@@ -3284,7 +3159,7 @@
         <v>1506629</v>
       </c>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>228</v>
       </c>
@@ -3313,7 +3188,7 @@
         <v>1467776</v>
       </c>
     </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>231</v>
       </c>
@@ -3342,7 +3217,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>234</v>
       </c>
@@ -3371,7 +3246,7 @@
         <v>2066354</v>
       </c>
     </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>240</v>
       </c>
@@ -3400,7 +3275,7 @@
         <v>2506414</v>
       </c>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>242</v>
       </c>
@@ -3429,7 +3304,7 @@
         <v>1903303</v>
       </c>
     </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>245</v>
       </c>
@@ -3458,7 +3333,7 @@
         <v>2212081</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>248</v>
       </c>
@@ -3487,7 +3362,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>253</v>
       </c>
@@ -3516,7 +3391,7 @@
         <v>2377140</v>
       </c>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>88</v>
       </c>
@@ -3545,7 +3420,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>260</v>
       </c>
@@ -3574,7 +3449,7 @@
         <v>2112373</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>262</v>
       </c>
@@ -3603,7 +3478,7 @@
         <v>2545845</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>264</v>
       </c>
@@ -3635,7 +3510,6 @@
         <v>276</v>
       </c>
     </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:J79">
     <filterColumn colId="0">
@@ -3701,11 +3575,6 @@
         <filter val="TCA6408A"/>
         <filter val="USB-B"/>
         <filter val="X1G004691000112"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="8">
-      <filters>
-        <filter val="2691054"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3779,1514 +3648,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId66"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I65"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="48.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="87.42578125" customWidth="1"/>
-    <col min="4" max="9" width="15.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="9">
-        <v>1</v>
-      </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>286</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="F3" s="9">
-        <v>20</v>
-      </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="9">
-        <v>5</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="9">
-        <v>1</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="9">
-        <v>2</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="9">
-        <v>2</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="9">
-        <v>2</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="9">
-        <v>5</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="9">
-        <v>2</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="9">
-        <v>4</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="9">
-        <v>7</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="9">
-        <v>5</v>
-      </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="9">
-        <v>1</v>
-      </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="9">
-        <v>1</v>
-      </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="9">
-        <v>2</v>
-      </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="9">
-        <v>1</v>
-      </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="F18" s="9">
-        <v>8</v>
-      </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="9">
-        <v>1</v>
-      </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="9">
-        <v>1</v>
-      </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="9">
-        <v>1</v>
-      </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="9">
-        <v>1</v>
-      </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F23" s="9">
-        <v>3</v>
-      </c>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="F24" s="9">
-        <v>1</v>
-      </c>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="F25" s="9">
-        <v>4</v>
-      </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F26" s="9">
-        <v>4</v>
-      </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>304</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>306</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="F27" s="9">
-        <v>1</v>
-      </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28" s="9">
-        <v>2</v>
-      </c>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="F29" s="9">
-        <v>1</v>
-      </c>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F30" s="9">
-        <v>2</v>
-      </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="F31" s="9">
-        <v>5</v>
-      </c>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="F32" s="9">
-        <v>1</v>
-      </c>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F33" s="9">
-        <v>1</v>
-      </c>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="F34" s="9">
-        <v>1</v>
-      </c>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>309</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="F35" s="9">
-        <v>1</v>
-      </c>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="F36" s="9">
-        <v>1</v>
-      </c>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
-        <v>750</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>309</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="F37" s="9">
-        <v>3</v>
-      </c>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="F38" s="9">
-        <v>3</v>
-      </c>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
-        <v>270</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="F39" s="9">
-        <v>1</v>
-      </c>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="F40" s="9">
-        <v>3</v>
-      </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="F41" s="9">
-        <v>2</v>
-      </c>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="F42" s="9">
-        <v>1</v>
-      </c>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
-        <v>51</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>320</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="F43" s="9">
-        <v>8</v>
-      </c>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="9">
-        <v>240</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="F44" s="9">
-        <v>1</v>
-      </c>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="9">
-        <v>30.1</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="F45" s="9">
-        <v>1</v>
-      </c>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="9">
-        <v>0</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="F46" s="9">
-        <v>1</v>
-      </c>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="F47" s="9">
-        <v>2</v>
-      </c>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="9">
-        <v>390</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F48" s="9">
-        <v>1</v>
-      </c>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="9">
-        <v>91</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="F49" s="9">
-        <v>1</v>
-      </c>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F50" s="9">
-        <v>1</v>
-      </c>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="F51" s="9">
-        <v>1</v>
-      </c>
-      <c r="G51" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="H51" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="I51" s="9"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="F52" s="9">
-        <v>1</v>
-      </c>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="F53" s="9">
-        <v>1</v>
-      </c>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="F54" s="9">
-        <v>1</v>
-      </c>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="F55" s="9">
-        <v>1</v>
-      </c>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="F56" s="9">
-        <v>1</v>
-      </c>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="F57" s="9">
-        <v>1</v>
-      </c>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="F58" s="9">
-        <v>1</v>
-      </c>
-      <c r="G58" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="F59" s="9">
-        <v>1</v>
-      </c>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9" t="s">
-        <v>322</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="F60" s="9">
-        <v>1</v>
-      </c>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="F61" s="9">
-        <v>1</v>
-      </c>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>323</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="F62" s="9">
-        <v>2</v>
-      </c>
-      <c r="G62" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="H62" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="I62" s="9"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F63" s="9">
-        <v>1</v>
-      </c>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="F64" s="9">
-        <v>1</v>
-      </c>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-      <c r="I64" s="9"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="F65" s="9">
-        <v>1</v>
-      </c>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
-      <c r="I65" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>